<commit_message>
Complete community stats parser
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24065</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -490,10 +490,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>75790</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H2" t="n">
         <v>17826</v>
@@ -510,7 +510,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,15 +554,40 @@
           <t>attend_times</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>solution</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>discuss</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>reputation</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>reput_level</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>jian-i6</t>
+          <t>JOHNKRAM</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1452</v>
+        <v>3584</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -571,62 +596,82 @@
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>清华大学</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Java</t>
+          <t>C++</t>
         </is>
       </c>
       <c r="H2" t="n">
         <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>19400</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Omega515</t>
+          <t>qeetcode</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1468</v>
+        <v>3257</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>VK</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>VK</t>
-        </is>
-      </c>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>UGTU</t>
+          <t>University of California--Berkeley</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>MySQL</t>
+          <t>C++</t>
         </is>
       </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
+      <c r="I3" t="n">
+        <v>119000</v>
+      </c>
+      <c r="J3" t="n">
+        <v>972</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>578</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>andywanghappy</t>
+          <t>bucketpotato</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1554</v>
+        <v>3169</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -635,28 +680,37 @@
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>haapy</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Java</t>
+          <t>C++</t>
         </is>
       </c>
       <c r="H4" t="n">
         <v>1</v>
       </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Blue_berry</t>
+          <t>moransky</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1361</v>
+        <v>3368</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -665,39 +719,54 @@
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>山东工商学院</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Java</t>
+          <t>C++</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>暂无</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>nayanshingare93</t>
+          <t>jinmingli</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1336</v>
+        <v>2997</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>高德地图</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>算法专家</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Fr. C. Rodrigues Institute of Technology.</t>
+          <t>清华大学</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -707,16 +776,27 @@
       </c>
       <c r="H6" t="n">
         <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>暂无</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>likhitha_560</t>
+          <t>galencolin</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1319</v>
+        <v>2817</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -734,53 +814,77 @@
       <c r="H7" t="n">
         <v>1</v>
       </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>valakondaanusha</t>
+          <t>lucifer1006</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1452</v>
+        <v>3097</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>China</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>NICE</t>
+          <t>Viktor Chondria University</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Researcher</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>College of Engineering Pune</t>
+          <t>北京大学</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Java</t>
+          <t>C++</t>
         </is>
       </c>
       <c r="H8" t="n">
         <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>暂无</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>samjohn4</t>
+          <t>nyu_ldf</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1354</v>
+        <v>3494</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -792,51 +896,79 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Python3</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="H9" t="n">
         <v>1</v>
       </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Jagan_45</t>
+          <t>liouzhou_101</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1343</v>
+        <v>3204</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>China</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>清华大学</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Python3</t>
+          <t>C++</t>
         </is>
       </c>
       <c r="H10" t="n">
         <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>暂无</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>mojadh</t>
+          <t>c8kbf</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1406</v>
+        <v>2923</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -850,19 +982,32 @@
       <c r="H11" t="n">
         <v>1</v>
       </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>a720732</t>
+          <t>raincoat911</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1452</v>
+        <v>2901</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -876,24 +1021,41 @@
       <c r="H12" t="n">
         <v>1</v>
       </c>
+      <c r="I12" t="n">
+        <v>405</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>5</v>
+      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>HooStax</t>
+          <t>delphih</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1322</v>
+        <v>2768</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Georgia Institute of Technology</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
         <is>
           <t>Python3</t>
@@ -902,24 +1064,41 @@
       <c r="H13" t="n">
         <v>1</v>
       </c>
+      <c r="I13" t="n">
+        <v>16400</v>
+      </c>
+      <c r="J13" t="n">
+        <v>29</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>219</v>
+      </c>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>The7thconqurer</t>
+          <t>arignote</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1452</v>
+        <v>3408</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>China</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>海外高校</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr">
         <is>
           <t>Java</t>
@@ -927,20 +1106,31 @@
       </c>
       <c r="H14" t="n">
         <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>暂无</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>priyanshupriyam123vv</t>
+          <t>lympanda</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1452</v>
+        <v>3139</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -948,21 +1138,34 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Python3</t>
+          <t>C++</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>1</v>
       </c>
+      <c r="I15" t="n">
+        <v>220</v>
+      </c>
+      <c r="J15" t="n">
+        <v>3</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>baisj</t>
+          <t>cpp_template</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1452</v>
+        <v>3104</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -971,11 +1174,7 @@
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>中南民族大学</t>
-        </is>
-      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
           <t>C++</t>
@@ -983,25 +1182,40 @@
       </c>
       <c r="H16" t="n">
         <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>暂无</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>mani_maestro1</t>
+          <t>Yawn_Sean</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1432</v>
+        <v>3118</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>China</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>北京大学</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr">
         <is>
           <t>Python3</t>
@@ -1009,20 +1223,31 @@
       </c>
       <c r="H17" t="n">
         <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>nmellert</t>
+          <t>Tlatoani</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1458</v>
+        <v>3225</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -1030,12 +1255,357 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
+          <t>Kotlin</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>user3754Ay</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2027</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Massachusetts Institute of Technology</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>bitetheD4T</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2756</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>浙大宁波理工学院</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>563</v>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>jianghd1996</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>2712</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>北京大学</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>Python</t>
         </is>
       </c>
-      <c r="H18" t="n">
-        <v>1</v>
-      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>暂无</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>lxhgww</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>2772</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>清华大学</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>暂无</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>sammochen</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>3049</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>University of Auckland</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>w285714</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2938</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>北京大学</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>暂无</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>uwi</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>3463</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Java</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>787</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>21</v>
+      </c>
+      <c r="M25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>ray_striker</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2500</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>National Institute of Technology, Silchar</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>5100</v>
+      </c>
+      <c r="J26" t="n">
+        <v>4</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" t="n">
+        <v>9</v>
+      </c>
+      <c r="M26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>